<commit_message>
Using char[2] instead of string for simplepricers
</commit_message>
<xml_diff>
--- a/Simple Barrier Pricing.xlsx
+++ b/Simple Barrier Pricing.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashish\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashish\Desktop\Princeton\Fall 2018\ORF 531 Computational Finance in C++\Group Project\Code\Group3-orflib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,58 +56,58 @@
     <t>uo</t>
   </si>
   <si>
+    <t>Option Fixed Properties</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Option Types</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>Call Price</t>
+  </si>
+  <si>
+    <t>Put Price</t>
+  </si>
+  <si>
+    <t>CUI</t>
+  </si>
+  <si>
+    <t>CUO</t>
+  </si>
+  <si>
+    <t>CDI</t>
+  </si>
+  <si>
+    <t>CDO</t>
+  </si>
+  <si>
+    <t>PUI</t>
+  </si>
+  <si>
+    <t>PUO</t>
+  </si>
+  <si>
+    <t>PDI</t>
+  </si>
+  <si>
+    <t>PDO</t>
+  </si>
+  <si>
+    <t>Barrier &gt; Strike</t>
+  </si>
+  <si>
+    <t>Barrier &lt;= Strike</t>
+  </si>
+  <si>
     <t>ui</t>
-  </si>
-  <si>
-    <t>Option Fixed Properties</t>
-  </si>
-  <si>
-    <t>Market</t>
-  </si>
-  <si>
-    <t>Option Types</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>Call Price</t>
-  </si>
-  <si>
-    <t>Put Price</t>
-  </si>
-  <si>
-    <t>CUI</t>
-  </si>
-  <si>
-    <t>CUO</t>
-  </si>
-  <si>
-    <t>CDI</t>
-  </si>
-  <si>
-    <t>CDO</t>
-  </si>
-  <si>
-    <t>PUI</t>
-  </si>
-  <si>
-    <t>PUO</t>
-  </si>
-  <si>
-    <t>PDI</t>
-  </si>
-  <si>
-    <t>PDO</t>
-  </si>
-  <si>
-    <t>Barrier &gt; Strike</t>
-  </si>
-  <si>
-    <t>Barrier &lt;= Strike</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H27" activeCellId="1" sqref="C28 H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,16 +486,16 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,14 +569,14 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <f>_xll.ORF.EUROBS(B3,$B$12,$B$8,$B$9,$B$13,$B$14,$B$15)</f>
         <v>6.7985644961671596</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18">
         <f>_xll.ORF.EUROBS(C3,$B$12,$B$8,$B$9,$B$13,$B$14,$B$15)</f>
@@ -585,15 +585,15 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <f>_xll.ORF.BARRBS(B3,B4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -606,7 +606,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <f>_xll.ORF.BARRBS(B3,C4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -619,7 +619,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <f>_xll.ORF.BARRBS(B3,D4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -632,7 +632,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <f>_xll.ORF.BARRBS(B3,E4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -645,7 +645,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26">
         <f>_xll.ORF.BARRBS(C3,B4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -658,7 +658,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3">
         <f>_xll.ORF.BARRBS(C3,C4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -671,7 +671,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <f>_xll.ORF.BARRBS(C3,D4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>
@@ -684,7 +684,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29">
         <f>_xll.ORF.BARRBS(C3,E4,$B$12,$B$8,$B$5,$B$9,$B$13,$B$14,$B$15)</f>

</xml_diff>